<commit_message>
upd norm JOYCITY-514: JOYCITY-512 уже лучше
</commit_message>
<xml_diff>
--- a/data/templates/test_order_data.xlsx
+++ b/data/templates/test_order_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasmi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\joycity_web_backend\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61367B-39A4-46A8-A113-343E05090842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1893A20D-D0D9-4E6B-B8D2-E7B515B346C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="405">
   <si>
     <t>Фото</t>
   </si>
@@ -1582,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,11 +1645,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1659,43 +1654,43 @@
           <x14:formula1>
             <xm:f>Справочники!$A$2:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C99</xm:sqref>
+          <xm:sqref>C2:C97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000063000000}">
           <x14:formula1>
             <xm:f>IF(C2="Женщинам",Справочники!$B$2:$B$28,IF(C2="Мужчинам",Справочники!$C$2:$C$28,IF(C2="Детям",Справочники!$D$2:$D$25,IF(C2="Обувь",Справочники!$J$2:$J$7,IF(C2="Дом",Справочники!$K$2:$K$23,IF(C2="Красота",Справочники!$L$2:$L$22,IF(C2="Аксессуары",Справочники!$M$2:$M$20,IF(C2="Электроника",Справочники!$N$2:$N$18,IF(C2="Игрушки",Справочники!$O$2:$O$23,IF(C2="Мебель",Справочники!$P$2:$P$19,IF(C2="Бытовая техника",Справочники!$Q$2:$Q$7,IF(C2="Зоотовары",Справочники!$R$2:$R$20,IF(C2="Спорт",Справочники!$S$2:$S$28,IF(C2="Автотовары",Справочники!$T$2:$T$18,IF(C2="Книги",Справочники!$U$2:$U$29,IF(C2="Ювелирные изделия",Справочники!$V$2:$V$17,IF(C2="Для ремонта",Справочники!$W$2:$W$11,IF(C2="Сад и дача",Справочники!$X$2:$X$21,IF(C2="Здоровье",Справочники!$Y$2:$Y$18,IF(C2="Канцтовары",Справочники!$Z$2:$Z$10,"Выберите категорию"))))))))))))))))))))</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D99</xm:sqref>
+          <xm:sqref>D2:D97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-0000C6000000}">
           <x14:formula1>
             <xm:f>Справочники!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H99</xm:sqref>
+          <xm:sqref>H2:H97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000029010000}">
           <x14:formula1>
             <xm:f>Справочники!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I99</xm:sqref>
+          <xm:sqref>I2:I97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00008C010000}">
           <x14:formula1>
             <xm:f>Справочники!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J99</xm:sqref>
+          <xm:sqref>J2:J97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-0000EF010000}">
           <x14:formula1>
             <xm:f>Справочники!$H$2:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K99</xm:sqref>
+          <xm:sqref>K2:K97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000052020000}">
           <x14:formula1>
             <xm:f>Справочники!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M99</xm:sqref>
+          <xm:sqref>M2:M97</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
upd norm JOYCITY-514: JOYCITY-512 norm
</commit_message>
<xml_diff>
--- a/data/templates/test_order_data.xlsx
+++ b/data/templates/test_order_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\joycity_web_backend\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasmi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1893A20D-D0D9-4E6B-B8D2-E7B515B346C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410AC13-25F7-4C3C-BC20-41C523A452B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1584,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,43 +1654,43 @@
           <x14:formula1>
             <xm:f>Справочники!$A$2:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C97</xm:sqref>
+          <xm:sqref>C2:C99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000063000000}">
           <x14:formula1>
             <xm:f>IF(C2="Женщинам",Справочники!$B$2:$B$28,IF(C2="Мужчинам",Справочники!$C$2:$C$28,IF(C2="Детям",Справочники!$D$2:$D$25,IF(C2="Обувь",Справочники!$J$2:$J$7,IF(C2="Дом",Справочники!$K$2:$K$23,IF(C2="Красота",Справочники!$L$2:$L$22,IF(C2="Аксессуары",Справочники!$M$2:$M$20,IF(C2="Электроника",Справочники!$N$2:$N$18,IF(C2="Игрушки",Справочники!$O$2:$O$23,IF(C2="Мебель",Справочники!$P$2:$P$19,IF(C2="Бытовая техника",Справочники!$Q$2:$Q$7,IF(C2="Зоотовары",Справочники!$R$2:$R$20,IF(C2="Спорт",Справочники!$S$2:$S$28,IF(C2="Автотовары",Справочники!$T$2:$T$18,IF(C2="Книги",Справочники!$U$2:$U$29,IF(C2="Ювелирные изделия",Справочники!$V$2:$V$17,IF(C2="Для ремонта",Справочники!$W$2:$W$11,IF(C2="Сад и дача",Справочники!$X$2:$X$21,IF(C2="Здоровье",Справочники!$Y$2:$Y$18,IF(C2="Канцтовары",Справочники!$Z$2:$Z$10,"Выберите категорию"))))))))))))))))))))</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D97</xm:sqref>
+          <xm:sqref>D2:D99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-0000C6000000}">
           <x14:formula1>
             <xm:f>Справочники!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H97</xm:sqref>
+          <xm:sqref>H2:H99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000029010000}">
           <x14:formula1>
             <xm:f>Справочники!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I97</xm:sqref>
+          <xm:sqref>I2:I99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00008C010000}">
           <x14:formula1>
             <xm:f>Справочники!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J97</xm:sqref>
+          <xm:sqref>J2:J99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-0000EF010000}">
           <x14:formula1>
             <xm:f>Справочники!$H$2:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K97</xm:sqref>
+          <xm:sqref>K2:K99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000052020000}">
           <x14:formula1>
             <xm:f>Справочники!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M97</xm:sqref>
+          <xm:sqref>M2:M99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>